<commit_message>
added helper sheet for validation of construction projects'
</commit_message>
<xml_diff>
--- a/dropdown_example.xlsx
+++ b/dropdown_example.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Dropdown Example" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,17 +413,26 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Select Option</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+  </sheetData>
   <dataValidations count="1">
-    <dataValidation sqref="B2:B10" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Apple,Banana,Orange,Grape"</formula1>
+    <dataValidation sqref="A2" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"0 - 10%: Foundation completed: Groundwork finished; no vertical structure yet.,11 - 25%: Structure and rough-in started: Structural framing in progress; initial MEP rough-in."</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>